<commit_message>
Added assets and modified the window code
</commit_message>
<xml_diff>
--- a/ClueGame/ClueBoard.xlsx
+++ b/ClueGame/ClueBoard.xlsx
@@ -1,20 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6CC18E00-2F6A-42E9-908A-9966081B4010}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,7 +116,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -583,11 +580,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>